<commit_message>
Bland-Altman plots and bootstrapping results added
</commit_message>
<xml_diff>
--- a/output/2023-05-11_WomenVAT1_visceral.adipose.tissue.valueAge_No.xlsx
+++ b/output/2023-05-11_WomenVAT1_visceral.adipose.tissue.valueAge_No.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmatth\Dropbox\Bodyscan_variable_selection\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5ABC4EA-37A2-4F8E-BACF-7F9485ED8E8F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27EB291E-B240-414C-A4EE-1C82F593E9CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13128" windowHeight="6108" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Percentage_inclusion" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="46">
   <si>
     <t/>
   </si>
@@ -499,9 +499,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -518,7 +518,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -535,7 +535,7 @@
         <v>39.799999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -552,7 +552,7 @@
         <v>37.204999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -569,7 +569,7 @@
         <v>53.302500000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -586,7 +586,7 @@
         <v>44.414999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -603,7 +603,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -620,7 +620,7 @@
         <v>49.902500000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -637,7 +637,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -654,7 +654,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -671,7 +671,7 @@
         <v>12.8025</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -688,7 +688,7 @@
         <v>4.4024999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -705,7 +705,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -722,7 +722,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -739,7 +739,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -756,7 +756,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -773,7 +773,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -790,7 +790,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -807,7 +807,7 @@
         <v>11.5025</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -824,7 +824,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -841,7 +841,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -858,7 +858,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -875,7 +875,7 @@
         <v>26.0075</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -892,7 +892,7 @@
         <v>27.9025</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -909,7 +909,7 @@
         <v>1.7024999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -926,7 +926,7 @@
         <v>1.1025</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -943,7 +943,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -960,7 +960,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -977,7 +977,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -994,7 +994,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -1059,9 +1059,9 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>37.204999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>44.414999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>12.8025</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>4.4024999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1214,7 +1214,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>11.5025</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1262,12 +1262,12 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -1299,7 +1299,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1555,7 +1555,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1619,7 +1619,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1651,7 +1651,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1715,7 +1715,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1747,7 +1747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -1779,7 +1779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1811,7 +1811,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -1999,7 +1999,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -2051,7 +2051,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -2129,7 +2129,7 @@
         <v>26.29</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -2155,7 +2155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -2215,19 +2215,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D15"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
@@ -2241,7 +2242,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -2255,7 +2256,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -2269,7 +2270,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -2283,7 +2284,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -2297,7 +2298,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
@@ -2311,7 +2312,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -2325,7 +2326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -2339,7 +2340,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -2353,7 +2354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -2367,7 +2368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -2380,30 +2381,6 @@
       <c r="D11" s="1">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>